<commit_message>
modify data tables UI and modify important notes with last updated date
</commit_message>
<xml_diff>
--- a/data/Administracion_de_viviendas_publicas/datos_vivienda.xlsx
+++ b/data/Administracion_de_viviendas_publicas/datos_vivienda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Administracion_de_viviendas_publicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEA08F2-107F-49A3-9443-6F9089AED87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B47C1E-6D21-48AF-A626-F80B89258D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="municipios_soli" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J79"/>
     </sheetView>
   </sheetViews>
@@ -3453,7 +3453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
@@ -5998,10 +5998,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6009,7 +6009,7 @@
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -6034,8 +6034,11 @@
       <c r="H1" s="1">
         <v>2023</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6060,8 +6063,11 @@
       <c r="H2">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6086,8 +6092,11 @@
       <c r="H3">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6112,8 +6121,11 @@
       <c r="H4">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6138,8 +6150,11 @@
       <c r="H5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -6164,8 +6179,11 @@
       <c r="H6">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6190,8 +6208,11 @@
       <c r="H7">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -6216,8 +6237,11 @@
       <c r="H8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -6242,8 +6266,11 @@
       <c r="H9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -6268,8 +6295,11 @@
       <c r="H10">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -6293,6 +6323,9 @@
       </c>
       <c r="H11">
         <v>17</v>
+      </c>
+      <c r="I11">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -6305,10 +6338,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6316,7 +6349,7 @@
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -6341,8 +6374,11 @@
       <c r="H1" s="1">
         <v>2023</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6367,8 +6403,11 @@
       <c r="H2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6393,8 +6432,11 @@
       <c r="H3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6419,8 +6461,11 @@
       <c r="H4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6445,8 +6490,11 @@
       <c r="H5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -6471,8 +6519,11 @@
       <c r="H6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6497,8 +6548,11 @@
       <c r="H7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -6523,8 +6577,11 @@
       <c r="H8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -6549,8 +6606,11 @@
       <c r="H9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -6575,8 +6635,11 @@
       <c r="H10">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -6600,6 +6663,9 @@
       </c>
       <c r="H11">
         <v>30</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>